<commit_message>
some more updates to variable list
</commit_message>
<xml_diff>
--- a/data/variables for model.xlsx
+++ b/data/variables for model.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>QB</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>for D: opponent's punk/kick returns allowed</t>
+  </si>
+  <si>
+    <t>historical salary of each player</t>
   </si>
 </sst>
 </file>
@@ -634,10 +637,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H38"/>
+  <dimension ref="B1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,6 +1166,11 @@
         <v>68</v>
       </c>
     </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="89" orientation="landscape" r:id="rId1"/>

</xml_diff>